<commit_message>
added adduct masses, glyco data, and small edits to parameter documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/Intact_Protein_Defaults.xlsx
+++ b/inst/extdata/Intact_Protein_Defaults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Git_Repos/ProteoMatch/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewi052/ProteoMatch/IsoMatchMS/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8977330F-07FF-714A-A208-57783F936A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE734BC4-0BB7-6E4D-AEB3-BB106B58F878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
-  <si>
-    <t>ProtonMass</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,9 +114,6 @@
     <t>Add most abundant isotope to the molecular formula calculation step. Warning: This will slow down the tool. </t>
   </si>
   <si>
-    <t>The AMU mass of a proton. Shouldn't need to change. </t>
-  </si>
-  <si>
     <t>2500-20000</t>
   </si>
   <si>
@@ -133,6 +127,21 @@
   </si>
   <si>
     <t xml:space="preserve"> 'closest peak' selects the closest peak in the m/z window (recommended for peptides/digested experiments/bottom-up/middle-down) and 'highest abundance' selects the highest abundance peak in the m/z window (recommended for intact protein/top-down)</t>
+  </si>
+  <si>
+    <t>AdductLabels</t>
+  </si>
+  <si>
+    <t>AdductMasses</t>
+  </si>
+  <si>
+    <t>proton</t>
+  </si>
+  <si>
+    <t>Labels for the AdductMasses. Should be separated by a comma with no space (ex. proton,sodium)</t>
+  </si>
+  <si>
+    <t>Masses for the Adducts. Should be separated by a comma with no space (ex. proton,sodium)</t>
   </si>
 </sst>
 </file>
@@ -168,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +200,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD1D1D1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD1D1D1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -207,6 +227,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -523,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25419109-B18E-184C-810E-4DA843070287}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,170 +562,184 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2">
         <v>2.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>0.5</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
         <v>1.0072764700000001</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Storing the return all parameter
</commit_message>
<xml_diff>
--- a/inst/extdata/Intact_Protein_Defaults.xlsx
+++ b/inst/extdata/Intact_Protein_Defaults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Git_Repos/IsoMatchMS/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85057F85-968D-A34A-AD42-0A54D4E2C54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A3D82D-8AD1-9743-9DD0-1EF750B10AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Parameter</t>
   </si>
@@ -108,9 +108,6 @@
     <t>AdductMasses</t>
   </si>
   <si>
-    <t>proton</t>
-  </si>
-  <si>
     <t>Labels for the AdductMasses. Should be separated by a comma with no space (ex. proton,sodium)</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve">Either "Rdisop" or "isopat". "Rdisop" is more accurate and recommended, though may crash on windows OS. "isopat" may then be used as an alternative. </t>
+  </si>
+  <si>
+    <t>proton,sodium,potassium</t>
+  </si>
+  <si>
+    <t>1.00727647,22.989769,39.0983</t>
   </si>
 </sst>
 </file>
@@ -493,13 +496,13 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="138.83203125" customWidth="1"/>
   </cols>
@@ -543,7 +546,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -562,7 +565,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>50</v>
@@ -571,7 +574,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,27 +610,27 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
-        <v>1.0072764700000001</v>
+      <c r="B9" t="s">
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -646,7 +649,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -655,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -674,16 +677,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>